<commit_message>
feat: handle apply api export/import file
</commit_message>
<xml_diff>
--- a/server/uploads/files/list-students.xlsx
+++ b/server/uploads/files/list-students.xlsx
@@ -1,10 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5889237E-7B6F-43F8-9CE7-8A56E7AAAF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="sheet 1" state="visible" r:id="rId4"/>
+    <sheet name="sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -22,17 +26,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -396,11 +402,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -410,6 +425,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>